<commit_message>
Use new plant filtering methodology in EDWP, edits to fix Capacity Price calculations and address achieved capacity factors (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B381C44-307E-49DE-954E-B30B7E9AB12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018F6EA-020B-4DA1-B7AB-BBF240326744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -800,7 +800,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +965,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3"/>
     </row>

</xml_diff>

<commit_message>
Implement new reliability-based capacity construction looping through hours in constructed timeslice (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018F6EA-020B-4DA1-B7AB-BBF240326744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2C5F1A-330D-4559-8108-D6F8ECDA20F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25185" yWindow="1770" windowWidth="28710" windowHeight="18495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>natural gas combined cycle</t>
   </si>
   <si>
-    <t>MCF Maximum Capacity Factor</t>
-  </si>
-  <si>
     <t>None needed</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>of electricity like wind and solar should not use maximum capacity factors.</t>
+  </si>
+  <si>
+    <t>BDTPTUMCF Boolean Does This Plant Type Use Maximum Capacity Factor</t>
   </si>
 </sst>
 </file>
@@ -719,9 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -733,7 +731,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -744,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1"/>
@@ -760,25 +758,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +798,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fix biomass+CCS and Sm Mod Reactor capacity factor alignment issues (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C25A3D4-6EB3-49FA-BEA0-CAE40DE0E920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C7DA66-C9AF-4876-A350-CFE923B8D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7455" yWindow="960" windowWidth="33780" windowHeight="21990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -221,12 +221,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -315,6 +321,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -815,13 +822,11 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -989,7 +994,8 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="9">
+        <f>B2</f>
         <v>1</v>
       </c>
     </row>
@@ -997,7 +1003,8 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="9">
+        <f>B4</f>
         <v>1</v>
       </c>
     </row>
@@ -1005,15 +1012,17 @@
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="8">
-        <v>1</v>
+      <c r="B21" s="9">
+        <f>B10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="9">
+        <f>B14</f>
         <v>1</v>
       </c>
     </row>
@@ -1021,8 +1030,9 @@
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="8">
-        <v>1</v>
+      <c r="B23" s="9">
+        <f>B5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates supporting economic dispatch of hydro plants
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446E642-D5F1-495A-9F7D-F6B45EF2F3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ED9A98-533A-401F-8B39-EF71FBE64D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -757,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -835,8 +835,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>

<commit_message>
Set negligible variable O&M costs for hydro so that it will run through least cost dispatch, lower HOC and disallow bidding at MCF in order to smooth hydro's dispatch
</commit_message>
<xml_diff>
--- a/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
+++ b/InputData/elec/BDTPTUMCF/Boolean Does This Plant Type Use Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BDTPTUMCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BDTPTUMCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ED9A98-533A-401F-8B39-EF71FBE64D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DCE9AD-342C-4F1D-9344-9510E0382F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="1695" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>